<commit_message>
Assets added for Milestone 3
</commit_message>
<xml_diff>
--- a/Documentation/Asset list.xlsx
+++ b/Documentation/Asset list.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\RIT2020SPRING\671\final\Elastic-Rush\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD2E8296-CC2B-4342-BEA7-1D72376E172E}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B4437D5-5CA8-4857-9672-1BCAC02C8961}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="61">
   <si>
     <t>Category</t>
   </si>
@@ -161,7 +161,67 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Ongoing</t>
+    <t>Added</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Alert sound on the top of the screen</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Ambience</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Sci-fi engine hovering sound scattering</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Future city surroundings</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Removed</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Sound effect</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Freeze gun pickup</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Gravity gun pickup</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Sonic gun pickup</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Gun reloading sound, faster</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Gun reloading sound, slower</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Weapon picking up sound</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Low pitch sci-fi digital sounds scattering</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Engine hovering</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Warnings</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -442,10 +502,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:D19"/>
+  <dimension ref="A1:D25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -578,7 +638,7 @@
         <v>18</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>45</v>
+        <v>50</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
@@ -676,7 +736,7 @@
         <v>33</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
@@ -690,7 +750,7 @@
         <v>36</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>41</v>
+        <v>50</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
@@ -719,6 +779,90 @@
       </c>
       <c r="D19" s="2" t="s">
         <v>41</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A23" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A24" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="D24" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A25" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="D25" s="2" t="s">
+        <v>45</v>
       </c>
     </row>
   </sheetData>

</xml_diff>